<commit_message>
Automatic merge of updates
</commit_message>
<xml_diff>
--- a/tfaip/scripts/xlsxexperimenter/example.xlsx
+++ b/tfaip/scripts/xlsxexperimenter/example.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">checkpoint_dir</t>
   </si>
   <si>
-    <t xml:space="preserve">train_batch_size</t>
+    <t xml:space="preserve">train.batch_size</t>
   </si>
   <si>
     <t xml:space="preserve">dataset</t>
@@ -222,10 +222,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.33"/>
@@ -237,7 +237,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="24.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.52"/>
@@ -338,10 +338,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J4" s="0" t="n">
         <v>10</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>500</v>
       </c>
       <c r="K4" s="0" t="str">
         <f aca="false">F4&amp;"_"&amp;G4</f>
@@ -387,10 +387,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J5" s="0" t="n">
         <v>10</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>500</v>
       </c>
       <c r="K5" s="0" t="str">
         <f aca="false">F5&amp;"_"&amp;G5</f>

</xml_diff>